<commit_message>
Issue #11112 - Inconsistent cruise names
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE09OSPM_00005.xlsx
+++ b/deployment/Omaha_Cal_Info_CE09OSPM_00005.xlsx
@@ -59,7 +59,7 @@
     <t>CE09OSPM-00005</t>
   </si>
   <si>
-    <t>TN342</t>
+    <t>TN-342</t>
   </si>
   <si>
     <t>Mooring Serial Number</t>
@@ -312,7 +312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -394,41 +394,41 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -452,28 +452,28 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,14 +492,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,7 +509,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -528,10 +528,10 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -561,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -579,7 +579,7 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -603,9 +603,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -614,9 +611,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -651,8 +645,8 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffccecff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="fffde9d9"/>
       <rgbColor rgb="ffff0000"/>
     </indexedColors>
@@ -805,9 +799,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -887,7 +881,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -915,10 +909,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1174,9 +1168,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1464,7 +1458,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1492,10 +1486,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2070,7 +2064,7 @@
       <c r="G3" t="s" s="27">
         <v>24</v>
       </c>
-      <c r="H3" s="31"/>
+      <c r="H3" s="7"/>
       <c r="I3" t="s" s="27">
         <v>25</v>
       </c>
@@ -2078,17 +2072,17 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="35"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" ht="16" customHeight="1">
       <c r="A5" t="s" s="27">
@@ -2109,10 +2103,10 @@
       <c r="F5" t="s" s="28">
         <v>28</v>
       </c>
-      <c r="G5" t="s" s="36">
+      <c r="G5" t="s" s="34">
         <v>29</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="7">
         <v>46.851277</v>
       </c>
       <c r="I5" s="7"/>
@@ -2138,10 +2132,10 @@
       <c r="F6" t="s" s="28">
         <v>28</v>
       </c>
-      <c r="G6" t="s" s="36">
+      <c r="G6" t="s" s="34">
         <v>30</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="7">
         <v>-124.982104</v>
       </c>
       <c r="I6" s="7"/>
@@ -2149,20 +2143,20 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" t="s" s="36">
+      <c r="A8" t="s" s="34">
         <v>31</v>
       </c>
       <c r="B8" t="s" s="27">
@@ -2183,7 +2177,7 @@
       <c r="G8" t="s" s="27">
         <v>29</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="7">
         <v>46.851277</v>
       </c>
       <c r="I8" s="7"/>
@@ -2191,7 +2185,7 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" t="s" s="36">
+      <c r="A9" t="s" s="34">
         <v>31</v>
       </c>
       <c r="B9" t="s" s="27">
@@ -2209,10 +2203,10 @@
       <c r="F9" t="s" s="30">
         <v>33</v>
       </c>
-      <c r="G9" t="s" s="36">
+      <c r="G9" t="s" s="34">
         <v>30</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="7">
         <v>-124.982104</v>
       </c>
       <c r="I9" s="7"/>
@@ -2220,7 +2214,7 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" t="s" s="36">
+      <c r="A10" t="s" s="34">
         <v>31</v>
       </c>
       <c r="B10" t="s" s="27">
@@ -2238,10 +2232,10 @@
       <c r="F10" t="s" s="30">
         <v>33</v>
       </c>
-      <c r="G10" t="s" s="36">
+      <c r="G10" t="s" s="34">
         <v>34</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="36">
         <v>0.00027191</v>
       </c>
       <c r="I10" t="s" s="27">
@@ -2251,7 +2245,7 @@
       <c r="K10" s="7"/>
     </row>
     <row r="11" ht="16" customHeight="1">
-      <c r="A11" t="s" s="36">
+      <c r="A11" t="s" s="34">
         <v>31</v>
       </c>
       <c r="B11" t="s" s="27">
@@ -2269,10 +2263,10 @@
       <c r="F11" t="s" s="30">
         <v>33</v>
       </c>
-      <c r="G11" t="s" s="36">
+      <c r="G11" t="s" s="34">
         <v>36</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="36">
         <v>-852.0204</v>
       </c>
       <c r="I11" s="7"/>
@@ -2280,7 +2274,7 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" ht="16" customHeight="1">
-      <c r="A12" t="s" s="36">
+      <c r="A12" t="s" s="34">
         <v>31</v>
       </c>
       <c r="B12" t="s" s="27">
@@ -2298,10 +2292,10 @@
       <c r="F12" t="s" s="30">
         <v>33</v>
       </c>
-      <c r="G12" t="s" s="36">
+      <c r="G12" t="s" s="34">
         <v>37</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H12" s="7">
         <v>-0.003828787</v>
       </c>
       <c r="I12" s="7"/>
@@ -2309,7 +2303,7 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" ht="16" customHeight="1">
-      <c r="A13" t="s" s="36">
+      <c r="A13" t="s" s="34">
         <v>31</v>
       </c>
       <c r="B13" t="s" s="27">
@@ -2327,10 +2321,10 @@
       <c r="F13" t="s" s="30">
         <v>33</v>
       </c>
-      <c r="G13" t="s" s="36">
+      <c r="G13" t="s" s="34">
         <v>38</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="36">
         <v>0.0001863749</v>
       </c>
       <c r="I13" s="7"/>
@@ -2338,7 +2332,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" ht="16" customHeight="1">
-      <c r="A14" t="s" s="36">
+      <c r="A14" t="s" s="34">
         <v>31</v>
       </c>
       <c r="B14" t="s" s="27">
@@ -2356,10 +2350,10 @@
       <c r="F14" t="s" s="30">
         <v>33</v>
       </c>
-      <c r="G14" t="s" s="36">
+      <c r="G14" t="s" s="34">
         <v>39</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="36">
         <v>-2.964531e-06</v>
       </c>
       <c r="I14" s="7"/>
@@ -2367,7 +2361,7 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" ht="16" customHeight="1">
-      <c r="A15" t="s" s="36">
+      <c r="A15" t="s" s="34">
         <v>31</v>
       </c>
       <c r="B15" t="s" s="27">
@@ -2385,10 +2379,10 @@
       <c r="F15" t="s" s="30">
         <v>33</v>
       </c>
-      <c r="G15" t="s" s="36">
+      <c r="G15" t="s" s="34">
         <v>40</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="36">
         <v>0.036</v>
       </c>
       <c r="I15" s="7"/>
@@ -2396,20 +2390,20 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" ht="16" customHeight="1">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="38"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
     <row r="17" ht="16" customHeight="1">
-      <c r="A17" t="s" s="36">
+      <c r="A17" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B17" t="s" s="27">
@@ -2430,7 +2424,7 @@
       <c r="G17" t="s" s="27">
         <v>43</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="7">
         <v>1.076</v>
       </c>
       <c r="I17" t="s" s="27">
@@ -2440,7 +2434,7 @@
       <c r="K17" s="7"/>
     </row>
     <row r="18" ht="16" customHeight="1">
-      <c r="A18" t="s" s="36">
+      <c r="A18" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B18" t="s" s="27">
@@ -2458,10 +2452,10 @@
       <c r="F18" s="29">
         <v>1030</v>
       </c>
-      <c r="G18" t="s" s="36">
+      <c r="G18" t="s" s="34">
         <v>45</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="7">
         <v>124</v>
       </c>
       <c r="I18" s="7"/>
@@ -2469,7 +2463,7 @@
       <c r="K18" s="7"/>
     </row>
     <row r="19" ht="16" customHeight="1">
-      <c r="A19" t="s" s="36">
+      <c r="A19" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B19" t="s" s="27">
@@ -2490,7 +2484,7 @@
       <c r="G19" t="s" s="27">
         <v>46</v>
       </c>
-      <c r="H19" s="35">
+      <c r="H19" s="7">
         <v>700</v>
       </c>
       <c r="I19" s="7"/>
@@ -2498,7 +2492,7 @@
       <c r="K19" s="7"/>
     </row>
     <row r="20" ht="16" customHeight="1">
-      <c r="A20" t="s" s="36">
+      <c r="A20" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B20" t="s" s="27">
@@ -2519,7 +2513,7 @@
       <c r="G20" t="s" s="27">
         <v>47</v>
       </c>
-      <c r="H20" s="35">
+      <c r="H20" s="7">
         <v>0.039</v>
       </c>
       <c r="I20" s="7"/>
@@ -2527,7 +2521,7 @@
       <c r="K20" s="7"/>
     </row>
     <row r="21" ht="16" customHeight="1">
-      <c r="A21" t="s" s="36">
+      <c r="A21" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B21" t="s" s="27">
@@ -2545,10 +2539,10 @@
       <c r="F21" s="29">
         <v>1030</v>
       </c>
-      <c r="G21" t="s" s="36">
+      <c r="G21" t="s" s="34">
         <v>48</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="35">
         <v>48</v>
       </c>
       <c r="I21" s="7"/>
@@ -2556,7 +2550,7 @@
       <c r="K21" s="7"/>
     </row>
     <row r="22" ht="16" customHeight="1">
-      <c r="A22" t="s" s="36">
+      <c r="A22" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B22" t="s" s="27">
@@ -2574,10 +2568,10 @@
       <c r="F22" s="29">
         <v>1030</v>
       </c>
-      <c r="G22" t="s" s="36">
+      <c r="G22" t="s" s="34">
         <v>49</v>
       </c>
-      <c r="H22" s="37">
+      <c r="H22" s="35">
         <v>3.308e-06</v>
       </c>
       <c r="I22" s="7"/>
@@ -2585,7 +2579,7 @@
       <c r="K22" s="7"/>
     </row>
     <row r="23" ht="16" customHeight="1">
-      <c r="A23" t="s" s="36">
+      <c r="A23" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B23" t="s" s="27">
@@ -2603,10 +2597,10 @@
       <c r="F23" s="29">
         <v>1030</v>
       </c>
-      <c r="G23" t="s" s="36">
+      <c r="G23" t="s" s="34">
         <v>50</v>
       </c>
-      <c r="H23" s="37">
+      <c r="H23" s="35">
         <v>48</v>
       </c>
       <c r="I23" s="7"/>
@@ -2614,7 +2608,7 @@
       <c r="K23" s="7"/>
     </row>
     <row r="24" ht="16" customHeight="1">
-      <c r="A24" t="s" s="36">
+      <c r="A24" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B24" t="s" s="27">
@@ -2632,10 +2626,10 @@
       <c r="F24" s="29">
         <v>1030</v>
       </c>
-      <c r="G24" t="s" s="36">
+      <c r="G24" t="s" s="34">
         <v>51</v>
       </c>
-      <c r="H24" s="37">
+      <c r="H24" s="35">
         <v>0.0699</v>
       </c>
       <c r="I24" s="7"/>
@@ -2643,7 +2637,7 @@
       <c r="K24" s="7"/>
     </row>
     <row r="25" ht="16" customHeight="1">
-      <c r="A25" t="s" s="36">
+      <c r="A25" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B25" t="s" s="27">
@@ -2661,10 +2655,10 @@
       <c r="F25" s="29">
         <v>1030</v>
       </c>
-      <c r="G25" t="s" s="36">
+      <c r="G25" t="s" s="34">
         <v>52</v>
       </c>
-      <c r="H25" s="37">
+      <c r="H25" s="35">
         <v>48</v>
       </c>
       <c r="I25" s="7"/>
@@ -2672,7 +2666,7 @@
       <c r="K25" s="7"/>
     </row>
     <row r="26" ht="16" customHeight="1">
-      <c r="A26" t="s" s="36">
+      <c r="A26" t="s" s="34">
         <v>41</v>
       </c>
       <c r="B26" t="s" s="27">
@@ -2690,10 +2684,10 @@
       <c r="F26" s="29">
         <v>1030</v>
       </c>
-      <c r="G26" t="s" s="36">
+      <c r="G26" t="s" s="34">
         <v>53</v>
       </c>
-      <c r="H26" s="37">
+      <c r="H26" s="35">
         <v>0.0121</v>
       </c>
       <c r="I26" s="7"/>
@@ -2701,20 +2695,20 @@
       <c r="K26" s="7"/>
     </row>
     <row r="27" ht="16" customHeight="1">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" ht="16" customHeight="1">
-      <c r="A28" t="s" s="36">
+      <c r="A28" t="s" s="34">
         <v>54</v>
       </c>
       <c r="B28" t="s" s="27">
@@ -2732,10 +2726,10 @@
       <c r="F28" s="29">
         <v>20438</v>
       </c>
-      <c r="G28" t="s" s="36">
+      <c r="G28" t="s" s="34">
         <v>56</v>
       </c>
-      <c r="H28" s="37">
+      <c r="H28" s="35">
         <v>1.1</v>
       </c>
       <c r="I28" t="s" s="27">
@@ -2745,7 +2739,7 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" ht="16" customHeight="1">
-      <c r="A29" t="s" s="36">
+      <c r="A29" t="s" s="34">
         <v>54</v>
       </c>
       <c r="B29" t="s" s="27">
@@ -2763,10 +2757,10 @@
       <c r="F29" s="29">
         <v>20438</v>
       </c>
-      <c r="G29" t="s" s="36">
+      <c r="G29" t="s" s="34">
         <v>58</v>
       </c>
-      <c r="H29" s="40">
+      <c r="H29" s="38">
         <v>1.03e-17</v>
       </c>
       <c r="I29" t="s" s="27">
@@ -2776,20 +2770,20 @@
       <c r="K29" s="7"/>
     </row>
     <row r="30" ht="16" customHeight="1">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="7"/>
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
       <c r="F30" s="19"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
     <row r="31" ht="16" customHeight="1">
-      <c r="A31" t="s" s="36">
+      <c r="A31" t="s" s="34">
         <v>60</v>
       </c>
       <c r="B31" t="s" s="27">
@@ -2804,13 +2798,13 @@
       <c r="E31" t="s" s="27">
         <v>61</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="37">
         <v>100014</v>
       </c>
-      <c r="G31" t="s" s="36">
+      <c r="G31" t="s" s="34">
         <v>29</v>
       </c>
-      <c r="H31" s="35">
+      <c r="H31" s="7">
         <v>46.851277</v>
       </c>
       <c r="I31" s="7"/>
@@ -2818,7 +2812,7 @@
       <c r="K31" s="7"/>
     </row>
     <row r="32" ht="16" customHeight="1">
-      <c r="A32" t="s" s="36">
+      <c r="A32" t="s" s="34">
         <v>60</v>
       </c>
       <c r="B32" t="s" s="27">
@@ -2833,13 +2827,13 @@
       <c r="E32" t="s" s="27">
         <v>61</v>
       </c>
-      <c r="F32" s="39">
+      <c r="F32" s="37">
         <v>100014</v>
       </c>
-      <c r="G32" t="s" s="36">
+      <c r="G32" t="s" s="34">
         <v>30</v>
       </c>
-      <c r="H32" s="35">
+      <c r="H32" s="7">
         <v>-124.982104</v>
       </c>
       <c r="I32" s="7"/>
@@ -2847,20 +2841,20 @@
       <c r="K32" s="7"/>
     </row>
     <row r="33" ht="16" customHeight="1">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
     <row r="34" ht="16" customHeight="1">
-      <c r="A34" t="s" s="36">
+      <c r="A34" t="s" s="34">
         <v>62</v>
       </c>
       <c r="B34" t="s" s="27">
@@ -2881,7 +2875,7 @@
       <c r="G34" t="s" s="27">
         <v>24</v>
       </c>
-      <c r="H34" s="35"/>
+      <c r="H34" s="7"/>
       <c r="I34" t="s" s="27">
         <v>65</v>
       </c>
@@ -2894,10 +2888,10 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>

</xml_diff>